<commit_message>
added benchmark to excel
</commit_message>
<xml_diff>
--- a/ASR Model results.xlsx
+++ b/ASR Model results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25003"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F6443F0-C8E9-488B-94CF-B82585999B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{18D69B00-C951-4E44-B19B-6EF3B6557874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="104">
   <si>
     <t>Demographic information for speakers with dysarthria</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -331,6 +331,21 @@
     <t>Word Recognition Accuracy</t>
   </si>
   <si>
+    <t>Speakers</t>
+  </si>
+  <si>
+    <t>Best Performing SD ASR in Baseline #1</t>
+  </si>
+  <si>
+    <t>Best Performing SD ASR in Baseline #2</t>
+  </si>
+  <si>
+    <t>Speech Vision</t>
+  </si>
+  <si>
+    <t>TransformerModel 2</t>
+  </si>
+  <si>
     <t>Before Transfer Learning</t>
   </si>
   <si>
@@ -362,6 +377,9 @@
   </si>
   <si>
     <t>High Intelligiblity Average WRA (%)</t>
+  </si>
+  <si>
+    <t>Absolute Average WRA (%)</t>
   </si>
 </sst>
 </file>
@@ -539,7 +557,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -593,9 +611,6 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -619,6 +634,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -668,6 +701,1526 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Benchmarking Speech vision's Word Recognition Accuracies (%)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'TransformerModel2.3 results'!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Best Performing SD ASR in Baseline #1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'TransformerModel2.3 results'!$G$3:$G$14</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>F03</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>M01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>M04</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>M12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>F02</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>M07</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>M16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>F04</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>M05</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>F05</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>M08</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>M09</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'TransformerModel2.3 results'!$H$3:$H$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.760000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.54</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32.24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>61.08</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>62.33</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64.290000000000006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>62.66</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>70.48</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>86.46</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>85.86</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>80.959999999999994</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-063C-4872-AF4B-95126959791C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'TransformerModel2.3 results'!$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Best Performing SD ASR in Baseline #2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'TransformerModel2.3 results'!$G$3:$G$14</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>F03</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>M01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>M04</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>M12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>F02</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>M07</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>M16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>F04</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>M05</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>F05</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>M08</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>M09</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'TransformerModel2.3 results'!$I$3:$I$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>17.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18.899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>66.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>53.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>53.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>56.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>85.6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>79.099999999999994</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-063C-4872-AF4B-95126959791C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'TransformerModel2.3 results'!$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Speech Vision</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'TransformerModel2.3 results'!$G$3:$G$14</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>F03</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>M01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>M04</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>M12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>F02</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>M07</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>M16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>F04</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>M05</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>F05</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>M08</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>M09</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'TransformerModel2.3 results'!$J$3:$J$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>32.47</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.39</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40.65</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>67.02</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>69.459999999999994</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>55.91</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>53.98</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>64.95</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>94.41</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>86.67</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>85.16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-063C-4872-AF4B-95126959791C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'TransformerModel2.3 results'!$K$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TransformerModel 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'TransformerModel2.3 results'!$G$3:$G$14</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>F03</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>M01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>M04</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>M12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>F02</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>M07</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>M16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>F04</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>M05</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>F05</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>M08</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>M09</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'TransformerModel2.3 results'!$K$3:$K$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>45.44</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35.049999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.5500000000000007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>38.71</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70.319999999999993</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>72.53</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>51.52</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>65.81</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>57.97</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>85.35</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>71.06</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>65.989999999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-063C-4872-AF4B-95126959791C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="119"/>
+        <c:axId val="578538632"/>
+        <c:axId val="97226951"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="578538632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="97226951"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="97226951"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="578538632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -712,6 +2265,47 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>828675</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1285875</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{257A6EC8-8B00-44F6-A991-44CB47A0B8D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1048,15 +2642,15 @@
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37"/>
-      <c r="T1" s="37"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="4"/>
@@ -1064,15 +2658,15 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="36"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="36"/>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="6"/>
@@ -1084,15 +2678,15 @@
         <v>2</v>
       </c>
       <c r="E3" s="6"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="38"/>
-      <c r="O3" s="38"/>
-      <c r="P3" s="38"/>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37"/>
-      <c r="S3" s="37"/>
-      <c r="T3" s="37"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="36"/>
+      <c r="R3" s="36"/>
+      <c r="S3" s="36"/>
+      <c r="T3" s="36"/>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" s="6" t="s">
@@ -1110,15 +2704,15 @@
       <c r="E4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="41"/>
-      <c r="M4" s="41"/>
-      <c r="N4" s="37"/>
-      <c r="O4" s="37"/>
-      <c r="P4" s="37"/>
-      <c r="Q4" s="37"/>
-      <c r="R4" s="37"/>
-      <c r="S4" s="37"/>
-      <c r="T4" s="37"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="36"/>
+      <c r="P4" s="36"/>
+      <c r="Q4" s="36"/>
+      <c r="R4" s="36"/>
+      <c r="S4" s="36"/>
+      <c r="T4" s="36"/>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" s="4"/>
@@ -1126,15 +2720,15 @@
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
-      <c r="L5" s="42"/>
-      <c r="M5" s="37"/>
-      <c r="N5" s="39"/>
-      <c r="O5" s="39"/>
-      <c r="P5" s="39"/>
-      <c r="Q5" s="37"/>
-      <c r="R5" s="37"/>
-      <c r="S5" s="37"/>
-      <c r="T5" s="37"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="36"/>
+      <c r="N5" s="38"/>
+      <c r="O5" s="38"/>
+      <c r="P5" s="38"/>
+      <c r="Q5" s="36"/>
+      <c r="R5" s="36"/>
+      <c r="S5" s="36"/>
+      <c r="T5" s="36"/>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" s="7" t="s">
@@ -1152,15 +2746,15 @@
       <c r="E6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="42"/>
-      <c r="M6" s="37"/>
-      <c r="N6" s="39"/>
-      <c r="O6" s="39"/>
-      <c r="P6" s="39"/>
-      <c r="Q6" s="37"/>
-      <c r="R6" s="37"/>
-      <c r="S6" s="37"/>
-      <c r="T6" s="37"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="38"/>
+      <c r="O6" s="38"/>
+      <c r="P6" s="38"/>
+      <c r="Q6" s="36"/>
+      <c r="R6" s="36"/>
+      <c r="S6" s="36"/>
+      <c r="T6" s="36"/>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" s="7"/>
@@ -1168,15 +2762,15 @@
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="4"/>
-      <c r="L7" s="42"/>
-      <c r="M7" s="37"/>
-      <c r="N7" s="39"/>
-      <c r="O7" s="39"/>
-      <c r="P7" s="39"/>
-      <c r="Q7" s="37"/>
-      <c r="R7" s="37"/>
-      <c r="S7" s="37"/>
-      <c r="T7" s="37"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="36"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="38"/>
+      <c r="P7" s="38"/>
+      <c r="Q7" s="36"/>
+      <c r="R7" s="36"/>
+      <c r="S7" s="36"/>
+      <c r="T7" s="36"/>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" s="7" t="s">
@@ -1194,15 +2788,15 @@
       <c r="E8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="42"/>
-      <c r="M8" s="37"/>
-      <c r="N8" s="39"/>
-      <c r="O8" s="39"/>
-      <c r="P8" s="39"/>
-      <c r="Q8" s="37"/>
-      <c r="R8" s="37"/>
-      <c r="S8" s="37"/>
-      <c r="T8" s="37"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="36"/>
+      <c r="N8" s="38"/>
+      <c r="O8" s="38"/>
+      <c r="P8" s="38"/>
+      <c r="Q8" s="36"/>
+      <c r="R8" s="36"/>
+      <c r="S8" s="36"/>
+      <c r="T8" s="36"/>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" s="7"/>
@@ -1210,15 +2804,15 @@
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="4"/>
-      <c r="L9" s="38"/>
-      <c r="M9" s="38"/>
-      <c r="N9" s="40"/>
-      <c r="O9" s="40"/>
-      <c r="P9" s="39"/>
-      <c r="Q9" s="37"/>
-      <c r="R9" s="37"/>
-      <c r="S9" s="37"/>
-      <c r="T9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="39"/>
+      <c r="O9" s="39"/>
+      <c r="P9" s="38"/>
+      <c r="Q9" s="36"/>
+      <c r="R9" s="36"/>
+      <c r="S9" s="36"/>
+      <c r="T9" s="36"/>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" s="7" t="s">
@@ -1236,15 +2830,15 @@
       <c r="E10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L10" s="43"/>
-      <c r="M10" s="37"/>
-      <c r="N10" s="39"/>
-      <c r="O10" s="39"/>
-      <c r="P10" s="39"/>
-      <c r="Q10" s="37"/>
-      <c r="R10" s="37"/>
-      <c r="S10" s="37"/>
-      <c r="T10" s="37"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="36"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="38"/>
+      <c r="P10" s="38"/>
+      <c r="Q10" s="36"/>
+      <c r="R10" s="36"/>
+      <c r="S10" s="36"/>
+      <c r="T10" s="36"/>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" s="7"/>
@@ -1252,15 +2846,15 @@
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="4"/>
-      <c r="L11" s="43"/>
-      <c r="M11" s="37"/>
-      <c r="N11" s="39"/>
-      <c r="O11" s="39"/>
-      <c r="P11" s="39"/>
-      <c r="Q11" s="37"/>
-      <c r="R11" s="37"/>
-      <c r="S11" s="37"/>
-      <c r="T11" s="37"/>
+      <c r="L11" s="42"/>
+      <c r="M11" s="36"/>
+      <c r="N11" s="38"/>
+      <c r="O11" s="38"/>
+      <c r="P11" s="38"/>
+      <c r="Q11" s="36"/>
+      <c r="R11" s="36"/>
+      <c r="S11" s="36"/>
+      <c r="T11" s="36"/>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="7" t="s">
@@ -1278,15 +2872,15 @@
       <c r="E12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L12" s="43"/>
-      <c r="M12" s="37"/>
-      <c r="N12" s="39"/>
-      <c r="O12" s="39"/>
-      <c r="P12" s="39"/>
-      <c r="Q12" s="37"/>
-      <c r="R12" s="37"/>
-      <c r="S12" s="37"/>
-      <c r="T12" s="37"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="36"/>
+      <c r="N12" s="38"/>
+      <c r="O12" s="38"/>
+      <c r="P12" s="38"/>
+      <c r="Q12" s="36"/>
+      <c r="R12" s="36"/>
+      <c r="S12" s="36"/>
+      <c r="T12" s="36"/>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="7"/>
@@ -1294,15 +2888,15 @@
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="4"/>
-      <c r="L13" s="38"/>
-      <c r="M13" s="38"/>
-      <c r="N13" s="40"/>
-      <c r="O13" s="40"/>
-      <c r="P13" s="39"/>
-      <c r="Q13" s="37"/>
-      <c r="R13" s="37"/>
-      <c r="S13" s="37"/>
-      <c r="T13" s="37"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="37"/>
+      <c r="N13" s="39"/>
+      <c r="O13" s="39"/>
+      <c r="P13" s="38"/>
+      <c r="Q13" s="36"/>
+      <c r="R13" s="36"/>
+      <c r="S13" s="36"/>
+      <c r="T13" s="36"/>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" s="7" t="s">
@@ -1320,15 +2914,15 @@
       <c r="E14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="43"/>
-      <c r="M14" s="37"/>
-      <c r="N14" s="39"/>
-      <c r="O14" s="39"/>
-      <c r="P14" s="39"/>
-      <c r="Q14" s="37"/>
-      <c r="R14" s="37"/>
-      <c r="S14" s="37"/>
-      <c r="T14" s="37"/>
+      <c r="L14" s="42"/>
+      <c r="M14" s="36"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="38"/>
+      <c r="P14" s="38"/>
+      <c r="Q14" s="36"/>
+      <c r="R14" s="36"/>
+      <c r="S14" s="36"/>
+      <c r="T14" s="36"/>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" s="7"/>
@@ -1336,15 +2930,15 @@
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="4"/>
-      <c r="L15" s="43"/>
-      <c r="M15" s="37"/>
-      <c r="N15" s="39"/>
-      <c r="O15" s="39"/>
-      <c r="P15" s="39"/>
-      <c r="Q15" s="37"/>
-      <c r="R15" s="37"/>
-      <c r="S15" s="37"/>
-      <c r="T15" s="37"/>
+      <c r="L15" s="42"/>
+      <c r="M15" s="36"/>
+      <c r="N15" s="38"/>
+      <c r="O15" s="38"/>
+      <c r="P15" s="38"/>
+      <c r="Q15" s="36"/>
+      <c r="R15" s="36"/>
+      <c r="S15" s="36"/>
+      <c r="T15" s="36"/>
     </row>
     <row r="16" spans="1:20">
       <c r="A16" s="7" t="s">
@@ -1362,15 +2956,15 @@
       <c r="E16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L16" s="38"/>
-      <c r="M16" s="38"/>
-      <c r="N16" s="40"/>
-      <c r="O16" s="40"/>
-      <c r="P16" s="39"/>
-      <c r="Q16" s="37"/>
-      <c r="R16" s="37"/>
-      <c r="S16" s="37"/>
-      <c r="T16" s="37"/>
+      <c r="L16" s="37"/>
+      <c r="M16" s="37"/>
+      <c r="N16" s="39"/>
+      <c r="O16" s="39"/>
+      <c r="P16" s="38"/>
+      <c r="Q16" s="36"/>
+      <c r="R16" s="36"/>
+      <c r="S16" s="36"/>
+      <c r="T16" s="36"/>
     </row>
     <row r="17" spans="1:20">
       <c r="A17" s="7"/>
@@ -1378,15 +2972,15 @@
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="4"/>
-      <c r="L17" s="43"/>
-      <c r="M17" s="37"/>
-      <c r="N17" s="39"/>
-      <c r="O17" s="39"/>
-      <c r="P17" s="39"/>
-      <c r="Q17" s="37"/>
-      <c r="R17" s="37"/>
-      <c r="S17" s="37"/>
-      <c r="T17" s="37"/>
+      <c r="L17" s="42"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="38"/>
+      <c r="O17" s="38"/>
+      <c r="P17" s="38"/>
+      <c r="Q17" s="36"/>
+      <c r="R17" s="36"/>
+      <c r="S17" s="36"/>
+      <c r="T17" s="36"/>
     </row>
     <row r="18" spans="1:20">
       <c r="A18" s="7" t="s">
@@ -1404,15 +2998,15 @@
       <c r="E18" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L18" s="43"/>
-      <c r="M18" s="37"/>
-      <c r="N18" s="39"/>
-      <c r="O18" s="39"/>
-      <c r="P18" s="39"/>
-      <c r="Q18" s="37"/>
-      <c r="R18" s="37"/>
-      <c r="S18" s="37"/>
-      <c r="T18" s="37"/>
+      <c r="L18" s="42"/>
+      <c r="M18" s="36"/>
+      <c r="N18" s="38"/>
+      <c r="O18" s="38"/>
+      <c r="P18" s="38"/>
+      <c r="Q18" s="36"/>
+      <c r="R18" s="36"/>
+      <c r="S18" s="36"/>
+      <c r="T18" s="36"/>
     </row>
     <row r="19" spans="1:20">
       <c r="A19" s="7"/>
@@ -1420,15 +3014,15 @@
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="4"/>
-      <c r="L19" s="43"/>
-      <c r="M19" s="37"/>
-      <c r="N19" s="39"/>
-      <c r="O19" s="39"/>
-      <c r="P19" s="39"/>
-      <c r="Q19" s="37"/>
-      <c r="R19" s="37"/>
-      <c r="S19" s="37"/>
-      <c r="T19" s="37"/>
+      <c r="L19" s="42"/>
+      <c r="M19" s="36"/>
+      <c r="N19" s="38"/>
+      <c r="O19" s="38"/>
+      <c r="P19" s="38"/>
+      <c r="Q19" s="36"/>
+      <c r="R19" s="36"/>
+      <c r="S19" s="36"/>
+      <c r="T19" s="36"/>
     </row>
     <row r="20" spans="1:20">
       <c r="A20" s="7" t="s">
@@ -1446,15 +3040,15 @@
       <c r="E20" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="L20" s="38"/>
-      <c r="M20" s="38"/>
-      <c r="N20" s="40"/>
-      <c r="O20" s="40"/>
-      <c r="P20" s="39"/>
-      <c r="Q20" s="37"/>
-      <c r="R20" s="37"/>
-      <c r="S20" s="37"/>
-      <c r="T20" s="37"/>
+      <c r="L20" s="37"/>
+      <c r="M20" s="37"/>
+      <c r="N20" s="39"/>
+      <c r="O20" s="39"/>
+      <c r="P20" s="38"/>
+      <c r="Q20" s="36"/>
+      <c r="R20" s="36"/>
+      <c r="S20" s="36"/>
+      <c r="T20" s="36"/>
     </row>
     <row r="21" spans="1:20">
       <c r="A21" s="7"/>
@@ -1462,15 +3056,15 @@
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="4"/>
-      <c r="L21" s="37"/>
-      <c r="M21" s="37"/>
-      <c r="N21" s="37"/>
-      <c r="O21" s="37"/>
-      <c r="P21" s="37"/>
-      <c r="Q21" s="37"/>
-      <c r="R21" s="37"/>
-      <c r="S21" s="37"/>
-      <c r="T21" s="37"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="36"/>
+      <c r="N21" s="36"/>
+      <c r="O21" s="36"/>
+      <c r="P21" s="36"/>
+      <c r="Q21" s="36"/>
+      <c r="R21" s="36"/>
+      <c r="S21" s="36"/>
+      <c r="T21" s="36"/>
     </row>
     <row r="22" spans="1:20">
       <c r="A22" s="7" t="s">
@@ -1488,15 +3082,15 @@
       <c r="E22" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L22" s="37"/>
-      <c r="M22" s="37"/>
-      <c r="N22" s="37"/>
-      <c r="O22" s="37"/>
-      <c r="P22" s="37"/>
-      <c r="Q22" s="37"/>
-      <c r="R22" s="37"/>
-      <c r="S22" s="37"/>
-      <c r="T22" s="37"/>
+      <c r="L22" s="36"/>
+      <c r="M22" s="36"/>
+      <c r="N22" s="36"/>
+      <c r="O22" s="36"/>
+      <c r="P22" s="36"/>
+      <c r="Q22" s="36"/>
+      <c r="R22" s="36"/>
+      <c r="S22" s="36"/>
+      <c r="T22" s="36"/>
     </row>
     <row r="23" spans="1:20">
       <c r="A23" s="7"/>
@@ -6011,215 +7605,215 @@
       </c>
     </row>
     <row r="163" spans="1:11">
-      <c r="A163" s="35"/>
-      <c r="B163" s="36"/>
-      <c r="C163" s="37"/>
-      <c r="D163" s="37"/>
-      <c r="E163" s="37"/>
+      <c r="A163" s="34"/>
+      <c r="B163" s="35"/>
+      <c r="C163" s="36"/>
+      <c r="D163" s="36"/>
+      <c r="E163" s="36"/>
       <c r="F163" s="26"/>
       <c r="G163" s="26"/>
     </row>
     <row r="164" spans="1:11">
-      <c r="A164" s="41"/>
-      <c r="B164" s="41"/>
-      <c r="C164" s="38"/>
-      <c r="D164" s="38"/>
-      <c r="E164" s="38"/>
+      <c r="A164" s="40"/>
+      <c r="B164" s="40"/>
+      <c r="C164" s="37"/>
+      <c r="D164" s="37"/>
+      <c r="E164" s="37"/>
       <c r="F164" s="26"/>
       <c r="G164" s="26"/>
     </row>
     <row r="165" spans="1:11">
-      <c r="A165" s="41"/>
-      <c r="B165" s="41"/>
-      <c r="C165" s="38"/>
-      <c r="D165" s="38"/>
-      <c r="E165" s="38"/>
+      <c r="A165" s="40"/>
+      <c r="B165" s="40"/>
+      <c r="C165" s="37"/>
+      <c r="D165" s="37"/>
+      <c r="E165" s="37"/>
       <c r="F165" s="26"/>
       <c r="G165" s="26"/>
     </row>
     <row r="166" spans="1:11">
-      <c r="A166" s="42"/>
-      <c r="B166" s="37"/>
-      <c r="C166" s="39"/>
-      <c r="D166" s="39"/>
-      <c r="E166" s="39"/>
+      <c r="A166" s="41"/>
+      <c r="B166" s="36"/>
+      <c r="C166" s="38"/>
+      <c r="D166" s="38"/>
+      <c r="E166" s="38"/>
       <c r="F166" s="26"/>
       <c r="G166" s="26"/>
     </row>
     <row r="167" spans="1:11">
-      <c r="A167" s="42"/>
-      <c r="B167" s="37"/>
-      <c r="C167" s="39"/>
-      <c r="D167" s="39"/>
-      <c r="E167" s="39"/>
+      <c r="A167" s="41"/>
+      <c r="B167" s="36"/>
+      <c r="C167" s="38"/>
+      <c r="D167" s="38"/>
+      <c r="E167" s="38"/>
       <c r="F167" s="26"/>
       <c r="G167" s="26"/>
     </row>
     <row r="168" spans="1:11">
-      <c r="A168" s="42"/>
-      <c r="B168" s="37"/>
-      <c r="C168" s="39"/>
-      <c r="D168" s="39"/>
-      <c r="E168" s="39"/>
+      <c r="A168" s="41"/>
+      <c r="B168" s="36"/>
+      <c r="C168" s="38"/>
+      <c r="D168" s="38"/>
+      <c r="E168" s="38"/>
       <c r="F168" s="26"/>
       <c r="G168" s="26"/>
     </row>
     <row r="169" spans="1:11">
-      <c r="A169" s="42"/>
-      <c r="B169" s="37"/>
-      <c r="C169" s="39"/>
-      <c r="D169" s="39"/>
-      <c r="E169" s="39"/>
+      <c r="A169" s="41"/>
+      <c r="B169" s="36"/>
+      <c r="C169" s="38"/>
+      <c r="D169" s="38"/>
+      <c r="E169" s="38"/>
       <c r="F169" s="26"/>
       <c r="G169" s="26"/>
     </row>
     <row r="170" spans="1:11">
-      <c r="A170" s="38"/>
-      <c r="B170" s="38"/>
-      <c r="C170" s="40"/>
-      <c r="D170" s="40"/>
-      <c r="E170" s="39"/>
+      <c r="A170" s="37"/>
+      <c r="B170" s="37"/>
+      <c r="C170" s="39"/>
+      <c r="D170" s="39"/>
+      <c r="E170" s="38"/>
       <c r="F170" s="26"/>
       <c r="G170" s="26"/>
     </row>
     <row r="171" spans="1:11">
-      <c r="A171" s="43"/>
-      <c r="B171" s="37"/>
-      <c r="C171" s="39"/>
-      <c r="D171" s="39"/>
-      <c r="E171" s="39"/>
+      <c r="A171" s="42"/>
+      <c r="B171" s="36"/>
+      <c r="C171" s="38"/>
+      <c r="D171" s="38"/>
+      <c r="E171" s="38"/>
       <c r="F171" s="26"/>
       <c r="G171" s="26"/>
     </row>
     <row r="172" spans="1:11">
-      <c r="A172" s="43"/>
-      <c r="B172" s="37"/>
-      <c r="C172" s="39"/>
-      <c r="D172" s="39"/>
-      <c r="E172" s="39"/>
+      <c r="A172" s="42"/>
+      <c r="B172" s="36"/>
+      <c r="C172" s="38"/>
+      <c r="D172" s="38"/>
+      <c r="E172" s="38"/>
       <c r="F172" s="26"/>
       <c r="G172" s="26"/>
     </row>
     <row r="173" spans="1:11">
-      <c r="A173" s="43"/>
-      <c r="B173" s="37"/>
-      <c r="C173" s="39"/>
-      <c r="D173" s="39"/>
-      <c r="E173" s="39"/>
+      <c r="A173" s="42"/>
+      <c r="B173" s="36"/>
+      <c r="C173" s="38"/>
+      <c r="D173" s="38"/>
+      <c r="E173" s="38"/>
       <c r="F173" s="26"/>
       <c r="G173" s="26"/>
     </row>
     <row r="174" spans="1:11">
-      <c r="A174" s="38"/>
-      <c r="B174" s="38"/>
-      <c r="C174" s="40"/>
-      <c r="D174" s="40"/>
-      <c r="E174" s="39"/>
+      <c r="A174" s="37"/>
+      <c r="B174" s="37"/>
+      <c r="C174" s="39"/>
+      <c r="D174" s="39"/>
+      <c r="E174" s="38"/>
       <c r="F174" s="26"/>
       <c r="G174" s="26"/>
     </row>
     <row r="175" spans="1:11">
-      <c r="A175" s="43"/>
-      <c r="B175" s="37"/>
-      <c r="C175" s="39"/>
-      <c r="D175" s="39"/>
-      <c r="E175" s="39"/>
+      <c r="A175" s="42"/>
+      <c r="B175" s="36"/>
+      <c r="C175" s="38"/>
+      <c r="D175" s="38"/>
+      <c r="E175" s="38"/>
       <c r="F175" s="26"/>
       <c r="G175" s="26"/>
     </row>
     <row r="176" spans="1:11">
-      <c r="A176" s="43"/>
-      <c r="B176" s="37"/>
-      <c r="C176" s="39"/>
-      <c r="D176" s="39"/>
-      <c r="E176" s="39"/>
+      <c r="A176" s="42"/>
+      <c r="B176" s="36"/>
+      <c r="C176" s="38"/>
+      <c r="D176" s="38"/>
+      <c r="E176" s="38"/>
       <c r="F176" s="26"/>
       <c r="G176" s="26"/>
     </row>
     <row r="177" spans="1:7">
-      <c r="A177" s="38"/>
-      <c r="B177" s="38"/>
-      <c r="C177" s="40"/>
-      <c r="D177" s="40"/>
-      <c r="E177" s="39"/>
+      <c r="A177" s="37"/>
+      <c r="B177" s="37"/>
+      <c r="C177" s="39"/>
+      <c r="D177" s="39"/>
+      <c r="E177" s="38"/>
       <c r="F177" s="26"/>
       <c r="G177" s="26"/>
     </row>
     <row r="178" spans="1:7">
-      <c r="A178" s="43"/>
-      <c r="B178" s="37"/>
-      <c r="C178" s="39"/>
-      <c r="D178" s="39"/>
-      <c r="E178" s="39"/>
+      <c r="A178" s="42"/>
+      <c r="B178" s="36"/>
+      <c r="C178" s="38"/>
+      <c r="D178" s="38"/>
+      <c r="E178" s="38"/>
       <c r="F178" s="26"/>
       <c r="G178" s="26"/>
     </row>
     <row r="179" spans="1:7">
-      <c r="A179" s="43"/>
-      <c r="B179" s="37"/>
-      <c r="C179" s="39"/>
-      <c r="D179" s="39"/>
-      <c r="E179" s="39"/>
+      <c r="A179" s="42"/>
+      <c r="B179" s="36"/>
+      <c r="C179" s="38"/>
+      <c r="D179" s="38"/>
+      <c r="E179" s="38"/>
       <c r="F179" s="26"/>
       <c r="G179" s="26"/>
     </row>
     <row r="180" spans="1:7">
-      <c r="A180" s="43"/>
-      <c r="B180" s="37"/>
-      <c r="C180" s="39"/>
-      <c r="D180" s="39"/>
-      <c r="E180" s="39"/>
+      <c r="A180" s="42"/>
+      <c r="B180" s="36"/>
+      <c r="C180" s="38"/>
+      <c r="D180" s="38"/>
+      <c r="E180" s="38"/>
       <c r="F180" s="26"/>
       <c r="G180" s="26"/>
     </row>
     <row r="181" spans="1:7">
-      <c r="A181" s="38"/>
-      <c r="B181" s="38"/>
-      <c r="C181" s="40"/>
-      <c r="D181" s="40"/>
-      <c r="E181" s="39"/>
+      <c r="A181" s="37"/>
+      <c r="B181" s="37"/>
+      <c r="C181" s="39"/>
+      <c r="D181" s="39"/>
+      <c r="E181" s="38"/>
       <c r="F181" s="26"/>
       <c r="G181" s="26"/>
     </row>
     <row r="182" spans="1:7">
-      <c r="A182" s="36"/>
-      <c r="B182" s="36"/>
-      <c r="C182" s="37"/>
-      <c r="D182" s="37"/>
-      <c r="E182" s="37"/>
+      <c r="A182" s="35"/>
+      <c r="B182" s="35"/>
+      <c r="C182" s="36"/>
+      <c r="D182" s="36"/>
+      <c r="E182" s="36"/>
       <c r="F182" s="26"/>
       <c r="G182" s="26"/>
     </row>
     <row r="183" spans="1:7">
-      <c r="A183" s="36"/>
-      <c r="B183" s="36"/>
-      <c r="C183" s="37"/>
-      <c r="D183" s="37"/>
-      <c r="E183" s="37"/>
+      <c r="A183" s="35"/>
+      <c r="B183" s="35"/>
+      <c r="C183" s="36"/>
+      <c r="D183" s="36"/>
+      <c r="E183" s="36"/>
       <c r="F183" s="26"/>
       <c r="G183" s="26"/>
     </row>
     <row r="184" spans="1:7">
-      <c r="A184" s="36"/>
-      <c r="B184" s="36"/>
-      <c r="C184" s="37"/>
-      <c r="D184" s="37"/>
-      <c r="E184" s="37"/>
+      <c r="A184" s="35"/>
+      <c r="B184" s="35"/>
+      <c r="C184" s="36"/>
+      <c r="D184" s="36"/>
+      <c r="E184" s="36"/>
       <c r="F184" s="26"/>
       <c r="G184" s="26"/>
     </row>
     <row r="185" spans="1:7">
-      <c r="A185" s="36"/>
-      <c r="B185" s="36"/>
-      <c r="C185" s="37"/>
-      <c r="D185" s="37"/>
-      <c r="E185" s="37"/>
+      <c r="A185" s="35"/>
+      <c r="B185" s="35"/>
+      <c r="C185" s="36"/>
+      <c r="D185" s="36"/>
+      <c r="E185" s="36"/>
       <c r="F185" s="26"/>
       <c r="G185" s="26"/>
     </row>
     <row r="186" spans="1:7">
-      <c r="A186" s="34"/>
-      <c r="B186" s="34"/>
+      <c r="A186" s="33"/>
+      <c r="B186" s="33"/>
       <c r="C186" s="26"/>
       <c r="D186" s="26"/>
       <c r="E186" s="26"/>
@@ -6363,7 +7957,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1DF05B8-ACCE-4DAE-9A03-F4ABDAFC8A20}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D11" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -6372,10 +7968,11 @@
     <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" style="26" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="35.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" style="26" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" style="26" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="26.28515625" customWidth="1"/>
     <col min="14" max="14" width="9.28515625" customWidth="1"/>
     <col min="15" max="15" width="23.140625" bestFit="1" customWidth="1"/>
@@ -6405,28 +8002,53 @@
       <c r="D2" s="13"/>
       <c r="E2" s="14"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
+      <c r="G2" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="I2" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="J2" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="K2" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="18"/>
       <c r="B3" s="10"/>
-      <c r="C3" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="E3" s="33" t="s">
-        <v>89</v>
+      <c r="C3" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" s="26">
+        <v>32</v>
+      </c>
+      <c r="I3" s="26">
+        <v>17.5</v>
+      </c>
+      <c r="J3" s="26">
+        <v>32.47</v>
+      </c>
+      <c r="K3" s="26">
+        <v>45.44</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="15" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B4" s="25" t="s">
         <v>69</v>
@@ -6440,6 +8062,21 @@
       <c r="E4" s="21">
         <f>(D4-C4)/C4</f>
         <v>4.4624746450305341E-2</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" s="26">
+        <v>16.760000000000002</v>
+      </c>
+      <c r="I4" s="26">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="J4" s="26">
+        <v>28.39</v>
+      </c>
+      <c r="K4" s="26">
+        <v>35.049999999999997</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -6457,6 +8094,21 @@
         <f t="shared" ref="E5:E19" si="0">(D5-C5)/C5</f>
         <v>-0.50920245398773034</v>
       </c>
+      <c r="G5" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="H5" s="26">
+        <v>6.54</v>
+      </c>
+      <c r="I5" s="26">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="J5" s="26">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="K5" s="26">
+        <v>9.5500000000000007</v>
+      </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="16"/>
@@ -6473,6 +8125,21 @@
         <f t="shared" si="0"/>
         <v>-0.52702702702702731</v>
       </c>
+      <c r="G6" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="H6" s="26">
+        <v>32.24</v>
+      </c>
+      <c r="I6" s="26">
+        <v>9</v>
+      </c>
+      <c r="J6" s="26">
+        <v>40.65</v>
+      </c>
+      <c r="K6" s="26">
+        <v>38.71</v>
+      </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="16"/>
@@ -6489,28 +8156,58 @@
         <f t="shared" si="0"/>
         <v>-0.68888888888889044</v>
       </c>
+      <c r="G7" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="H7" s="26">
+        <v>61.08</v>
+      </c>
+      <c r="I7" s="26">
+        <v>29.6</v>
+      </c>
+      <c r="J7" s="26">
+        <v>67.02</v>
+      </c>
+      <c r="K7" s="26">
+        <v>70.319999999999993</v>
+      </c>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="27" t="s">
-        <v>91</v>
-      </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="29">
+      <c r="A8" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" s="27"/>
+      <c r="C8" s="28">
         <f>AVERAGE(C4:C7)</f>
         <v>0.32187403993855573</v>
       </c>
-      <c r="D8" s="30">
+      <c r="D8" s="29">
         <f>AVERAGE(D4:D7)</f>
         <v>0.2030721966205834</v>
       </c>
-      <c r="E8" s="31">
+      <c r="E8" s="30">
         <f t="shared" si="0"/>
         <v>-0.36909420635678186</v>
       </c>
+      <c r="G8" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="H8" s="26">
+        <v>62.33</v>
+      </c>
+      <c r="I8" s="26">
+        <v>66.400000000000006</v>
+      </c>
+      <c r="J8" s="26">
+        <v>69.459999999999994</v>
+      </c>
+      <c r="K8" s="26">
+        <v>72.53</v>
+      </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="17" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B9" s="26" t="s">
         <v>81</v>
@@ -6524,6 +8221,21 @@
       <c r="E9" s="24">
         <f t="shared" si="0"/>
         <v>-0.17562254259501925</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="H9" s="26">
+        <v>64.290000000000006</v>
+      </c>
+      <c r="I9" s="26">
+        <v>53.6</v>
+      </c>
+      <c r="J9" s="26">
+        <v>55.91</v>
+      </c>
+      <c r="K9" s="26">
+        <v>51.52</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -6541,6 +8253,21 @@
         <f t="shared" si="0"/>
         <v>-0.36213468869123311</v>
       </c>
+      <c r="G10" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10" s="26">
+        <v>62.66</v>
+      </c>
+      <c r="I10" s="26">
+        <v>53.7</v>
+      </c>
+      <c r="J10" s="26">
+        <v>53.98</v>
+      </c>
+      <c r="K10" s="26">
+        <v>65.81</v>
+      </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="17"/>
@@ -6557,28 +8284,58 @@
         <f t="shared" si="0"/>
         <v>-0.19318181818181912</v>
       </c>
+      <c r="G11" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="H11" s="26">
+        <v>70.48</v>
+      </c>
+      <c r="I11" s="26">
+        <v>56.4</v>
+      </c>
+      <c r="J11" s="26">
+        <v>64.95</v>
+      </c>
+      <c r="K11" s="26">
+        <v>57.97</v>
+      </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="B12" s="28"/>
-      <c r="C12" s="29">
+      <c r="A12" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" s="27"/>
+      <c r="C12" s="28">
         <f>AVERAGE(C9:C11)</f>
         <v>0.64793130366900797</v>
       </c>
-      <c r="D12" s="30">
+      <c r="D12" s="29">
         <f>AVERAGE(D9:D11)</f>
         <v>0.48602905995819734</v>
       </c>
-      <c r="E12" s="31">
+      <c r="E12" s="30">
         <f t="shared" si="0"/>
         <v>-0.24987563155849232</v>
       </c>
+      <c r="G12" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="H12" s="26">
+        <v>86.46</v>
+      </c>
+      <c r="I12" s="26">
+        <v>85.6</v>
+      </c>
+      <c r="J12" s="26">
+        <v>94.41</v>
+      </c>
+      <c r="K12" s="26">
+        <v>85.35</v>
+      </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="17" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="B13" s="26" t="s">
         <v>71</v>
@@ -6592,6 +8349,21 @@
       <c r="E13" s="24">
         <f t="shared" si="0"/>
         <v>0.61538461538461464</v>
+      </c>
+      <c r="G13" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="H13" s="26">
+        <v>85.86</v>
+      </c>
+      <c r="I13" s="26">
+        <v>85</v>
+      </c>
+      <c r="J13" s="26">
+        <v>86.67</v>
+      </c>
+      <c r="K13" s="26">
+        <v>71.06</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -6609,28 +8381,43 @@
         <f t="shared" si="0"/>
         <v>-0.36565977742448447</v>
       </c>
+      <c r="G14" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="H14" s="26">
+        <v>80.959999999999994</v>
+      </c>
+      <c r="I14" s="26">
+        <v>79.099999999999994</v>
+      </c>
+      <c r="J14" s="26">
+        <v>85.16</v>
+      </c>
+      <c r="K14" s="26">
+        <v>65.989999999999995</v>
+      </c>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="B15" s="28"/>
-      <c r="C15" s="29">
+      <c r="A15" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="B15" s="27"/>
+      <c r="C15" s="28">
         <f>AVERAGE(C13:C14)</f>
         <v>0.49354838709677401</v>
       </c>
-      <c r="D15" s="30">
+      <c r="D15" s="29">
         <f>AVERAGE(D13:D14)</f>
         <v>0.51290322580645098</v>
       </c>
-      <c r="E15" s="31">
+      <c r="E15" s="30">
         <f t="shared" si="0"/>
         <v>3.9215686274508908E-2</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="17" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="B16" s="26" t="s">
         <v>72</v>
@@ -6679,25 +8466,40 @@
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="B19" s="28"/>
-      <c r="C19" s="29">
+      <c r="A19" s="50" t="s">
+        <v>102</v>
+      </c>
+      <c r="B19" s="45"/>
+      <c r="C19" s="46">
         <f>AVERAGE(C16:C18)</f>
         <v>0.69155145929339434</v>
       </c>
-      <c r="D19" s="30">
+      <c r="D19" s="47">
         <f>AVERAGE(D16:D18)</f>
         <v>0.71182795698924661</v>
       </c>
-      <c r="E19" s="31">
+      <c r="E19" s="21">
         <f t="shared" si="0"/>
         <v>2.9320302087960541E-2</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="B20" s="1"/>
+      <c r="A20" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="B20" s="48"/>
+      <c r="C20" s="29">
+        <f>AVERAGE(C19, C15, C12, C8)</f>
+        <v>0.53872629749943302</v>
+      </c>
+      <c r="D20" s="29">
+        <f t="shared" ref="D20" si="1">AVERAGE(D19, D15, D12, D8)</f>
+        <v>0.47845810984361958</v>
+      </c>
+      <c r="E20" s="44">
+        <f>(D20-C20)/C20</f>
+        <v>-0.11187162745823979</v>
+      </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1"/>
@@ -6722,10 +8524,11 @@
       <c r="B26" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="C2:E2"/>
+    <mergeCell ref="A20:B20"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="A4:A7"/>
@@ -6793,5 +8596,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>